<commit_message>
Implemented and tested maze calc and placement. Corrected ant debug.
</commit_message>
<xml_diff>
--- a/Server_files/plugins/DunGen/Module_Coordinates.xlsx
+++ b/Server_files/plugins/DunGen/Module_Coordinates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="24">
   <si>
     <t>Raum mit Säulen</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>passageWay Falling test</t>
+  </si>
+  <si>
+    <t>MazeTest</t>
+  </si>
+  <si>
+    <t>toMaze1</t>
+  </si>
+  <si>
+    <t>toMaze2</t>
+  </si>
+  <si>
+    <t>mazeEntry</t>
+  </si>
+  <si>
+    <t>mazeExit</t>
+  </si>
+  <si>
+    <t>goalCorn1</t>
+  </si>
+  <si>
+    <t>goalCorn2</t>
   </si>
 </sst>
 </file>
@@ -461,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AK27"/>
+  <dimension ref="C3:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AJ26" sqref="AJ26"/>
+    <sheetView tabSelected="1" topLeftCell="R10" workbookViewId="0">
+      <selection activeCell="AO41" sqref="AO41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +493,7 @@
     <col min="27" max="27" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -515,8 +536,15 @@
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5"/>
-    </row>
-    <row r="5" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+    </row>
+    <row r="5" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -551,8 +579,14 @@
       <c r="AI5" s="2">
         <v>1131</v>
       </c>
-    </row>
-    <row r="6" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AN5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="6" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -611,8 +645,18 @@
         <v>78</v>
       </c>
       <c r="AJ6" s="3"/>
-    </row>
-    <row r="7" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>64</v>
+      </c>
+      <c r="AP6" s="3"/>
+    </row>
+    <row r="7" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>4</v>
@@ -653,16 +697,24 @@
       <c r="AI7" s="2">
         <v>-223</v>
       </c>
-    </row>
-    <row r="8" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM7" s="1"/>
+      <c r="AN7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>-246</v>
+      </c>
+    </row>
+    <row r="8" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
       <c r="U8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AG8" s="1"/>
-    </row>
-    <row r="9" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM8" s="1"/>
+    </row>
+    <row r="9" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>2</v>
@@ -727,8 +779,19 @@
         <f>AI9-AI$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM9" s="1"/>
+      <c r="AN9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>957</v>
+      </c>
+      <c r="AQ9" s="4">
+        <f>AO9-AO$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -823,8 +886,24 @@
         <f>AI10-AI$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ10" s="4">
+        <f>AO10-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>4</v>
@@ -889,16 +968,28 @@
         <f>AI11-AI$7</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM11" s="1"/>
+      <c r="AN11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>-236</v>
+      </c>
+      <c r="AQ11" s="4">
+        <f>AO11-AO$7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
       <c r="U12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AG12" s="1"/>
-    </row>
-    <row r="13" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM12" s="1"/>
+    </row>
+    <row r="13" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>2</v>
@@ -963,8 +1054,19 @@
         <f>AI13-AI$5</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM13" s="1"/>
+      <c r="AN13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>980</v>
+      </c>
+      <c r="AQ13" s="4">
+        <f>AO13-AO$5</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1059,8 +1161,24 @@
         <f>AI14-AI$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ14" s="4">
+        <f>AO14-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>4</v>
@@ -1125,16 +1243,28 @@
         <f>AI15-AI$7</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM15" s="1"/>
+      <c r="AN15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO15" s="2">
+        <v>-233</v>
+      </c>
+      <c r="AQ15" s="4">
+        <f>AO15-AO$7</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
       <c r="U16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AG16" s="1"/>
-    </row>
-    <row r="17" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM16" s="1"/>
+    </row>
+    <row r="17" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>2</v>
@@ -1194,8 +1324,18 @@
         <f>AI17-AI$5</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AN17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO17" s="2">
+        <v>959</v>
+      </c>
+      <c r="AQ17" s="4">
+        <f>AO17-AO$5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1290,8 +1430,24 @@
         <f>AI18-AI$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO18" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ18" s="4">
+        <f>AO18-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
         <v>4</v>
@@ -1351,11 +1507,21 @@
         <f>AI19-AI$7</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AN19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO19" s="2">
+        <v>-245</v>
+      </c>
+      <c r="AQ19" s="4">
+        <f>AO19-AO$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" t="s">
         <v>2</v>
@@ -1377,8 +1543,18 @@
         <f>AC21-AC$5</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AN21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO21" s="2">
+        <v>978</v>
+      </c>
+      <c r="AQ21" s="4">
+        <f>AO21-AO$5</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1413,8 +1589,24 @@
         <v>4</v>
       </c>
       <c r="AJ22" s="3"/>
-    </row>
-    <row r="23" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO22" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ22" s="4">
+        <f>AO22-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -1435,8 +1627,18 @@
         <f>AC23-AC$7</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AN23" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO23" s="2">
+        <v>-226</v>
+      </c>
+      <c r="AQ23" s="4">
+        <f>AO23-AO$7</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="3:43" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
         <v>2</v>
       </c>
@@ -1447,8 +1649,18 @@
         <f>AC25-AC$5</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AN25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO25" s="2">
+        <v>958</v>
+      </c>
+      <c r="AQ25" s="4">
+        <f>AO25-AO$5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:43" x14ac:dyDescent="0.25">
       <c r="AA26" s="1" t="s">
         <v>14</v>
       </c>
@@ -1466,8 +1678,24 @@
         <v>4</v>
       </c>
       <c r="AJ26" s="3"/>
-    </row>
-    <row r="27" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="AM26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO26" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ26" s="4">
+        <f>AO26-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:43" x14ac:dyDescent="0.25">
       <c r="AB27" t="s">
         <v>4</v>
       </c>
@@ -1478,15 +1706,152 @@
         <f>AC27-AC$7</f>
         <v>9</v>
       </c>
+      <c r="AN27" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO27" s="2">
+        <v>-236</v>
+      </c>
+      <c r="AQ27" s="4">
+        <f>AO27-AO$7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AN29" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO29" s="2">
+        <v>979</v>
+      </c>
+      <c r="AQ29" s="4">
+        <f>AO29-AO$5</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AM30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO30" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ30" s="4">
+        <f>AO30-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AN31" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO31" s="2">
+        <v>-233</v>
+      </c>
+      <c r="AQ31" s="4">
+        <f>AO31-AO$7</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="39:43" x14ac:dyDescent="0.25">
+      <c r="AN34" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO34" s="2">
+        <v>979</v>
+      </c>
+      <c r="AQ34" s="4">
+        <f>AO34-AO$5</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="39:43" x14ac:dyDescent="0.25">
+      <c r="AM35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO35" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ35" s="4">
+        <f>AO35-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="39:43" x14ac:dyDescent="0.25">
+      <c r="AN36" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO36" s="2">
+        <v>-233</v>
+      </c>
+      <c r="AQ36" s="4">
+        <f>AO36-AO$7</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="39:43" x14ac:dyDescent="0.25">
+      <c r="AN38" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO38" s="2">
+        <v>979</v>
+      </c>
+      <c r="AQ38" s="4">
+        <f>AO38-AO$5</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="39:43" x14ac:dyDescent="0.25">
+      <c r="AM39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO39" s="2">
+        <v>65</v>
+      </c>
+      <c r="AP39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ39" s="4">
+        <f>AO39-AO$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="39:43" x14ac:dyDescent="0.25">
+      <c r="AN40" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO40" s="2">
+        <v>-232</v>
+      </c>
+      <c r="AQ40" s="4">
+        <f>AO40-AO$7</f>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="AM3:AQ3"/>
     <mergeCell ref="AG3:AK3"/>
     <mergeCell ref="U3:Y3"/>
     <mergeCell ref="O3:S3"/>
     <mergeCell ref="I3:M3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="AA3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Magma-Cave and Crater
</commit_message>
<xml_diff>
--- a/Server_files/plugins/DunGen/Module_Coordinates.xlsx
+++ b/Server_files/plugins/DunGen/Module_Coordinates.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="25">
   <si>
     <t>Raum mit Säulen</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>goalCorn2</t>
+  </si>
+  <si>
+    <t>Krater</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AQ40"/>
+  <dimension ref="C3:BC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R10" workbookViewId="0">
-      <selection activeCell="AO41" sqref="AO41"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="BA26" sqref="BA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +496,7 @@
     <col min="27" max="27" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -543,8 +546,22 @@
       <c r="AO3" s="5"/>
       <c r="AP3" s="5"/>
       <c r="AQ3" s="5"/>
-    </row>
-    <row r="5" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="5"/>
+      <c r="AU3" s="5"/>
+      <c r="AV3" s="5"/>
+      <c r="AW3" s="5"/>
+      <c r="AY3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AZ3" s="5"/>
+      <c r="BA3" s="5"/>
+      <c r="BB3" s="5"/>
+      <c r="BC3" s="5"/>
+    </row>
+    <row r="5" spans="3:55" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -585,8 +602,20 @@
       <c r="AO5" s="2">
         <v>957</v>
       </c>
-    </row>
-    <row r="6" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AT5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>1070</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA5" s="2">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="6" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -655,8 +684,28 @@
         <v>64</v>
       </c>
       <c r="AP6" s="3"/>
-    </row>
-    <row r="7" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>73</v>
+      </c>
+      <c r="AV6" s="3"/>
+      <c r="AY6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>84</v>
+      </c>
+      <c r="BB6" s="3"/>
+    </row>
+    <row r="7" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>4</v>
@@ -704,8 +753,22 @@
       <c r="AO7" s="2">
         <v>-246</v>
       </c>
-    </row>
-    <row r="8" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS7" s="1"/>
+      <c r="AT7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>-6</v>
+      </c>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>-453</v>
+      </c>
+    </row>
+    <row r="8" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
@@ -713,8 +776,10 @@
       <c r="AA8" s="1"/>
       <c r="AG8" s="1"/>
       <c r="AM8" s="1"/>
-    </row>
-    <row r="9" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS8" s="1"/>
+      <c r="AY8" s="1"/>
+    </row>
+    <row r="9" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>2</v>
@@ -790,8 +855,30 @@
         <f>AO9-AO$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS9" s="1"/>
+      <c r="AT9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU9" s="2">
+        <v>1070</v>
+      </c>
+      <c r="AW9" s="4">
+        <f>AU9-AU$5</f>
+        <v>0</v>
+      </c>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA9" s="2">
+        <v>1391</v>
+      </c>
+      <c r="BC9" s="4">
+        <f>BA9-BA$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -902,8 +989,40 @@
         <f>AO10-AO$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU10" s="2">
+        <v>80</v>
+      </c>
+      <c r="AV10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW10" s="4">
+        <f>AU10-AU$6</f>
+        <v>7</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA10" s="2">
+        <v>86</v>
+      </c>
+      <c r="BB10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC10" s="4">
+        <f>BA10-BA$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>4</v>
@@ -979,8 +1098,30 @@
         <f>AO11-AO$7</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS11" s="1"/>
+      <c r="AT11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU11" s="2">
+        <v>4</v>
+      </c>
+      <c r="AW11" s="4">
+        <f>AU11-AU$7</f>
+        <v>10</v>
+      </c>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA11" s="2">
+        <v>-398</v>
+      </c>
+      <c r="BC11" s="4">
+        <f>BA11-BA$7</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
@@ -988,8 +1129,10 @@
       <c r="AA12" s="1"/>
       <c r="AG12" s="1"/>
       <c r="AM12" s="1"/>
-    </row>
-    <row r="13" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS12" s="1"/>
+      <c r="AY12" s="1"/>
+    </row>
+    <row r="13" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>2</v>
@@ -1065,8 +1208,30 @@
         <f>AO13-AO$5</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS13" s="1"/>
+      <c r="AT13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU13" s="2">
+        <v>1090</v>
+      </c>
+      <c r="AW13" s="4">
+        <f>AU13-AU$5</f>
+        <v>20</v>
+      </c>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA13" s="2">
+        <v>1492</v>
+      </c>
+      <c r="BC13" s="4">
+        <f>BA13-BA$5</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1177,8 +1342,40 @@
         <f>AO14-AO$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU14" s="2">
+        <v>80</v>
+      </c>
+      <c r="AV14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW14" s="4">
+        <f>AU14-AU$6</f>
+        <v>7</v>
+      </c>
+      <c r="AY14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA14" s="2">
+        <v>86</v>
+      </c>
+      <c r="BB14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC14" s="4">
+        <f>BA14-BA$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>4</v>
@@ -1254,8 +1451,30 @@
         <f>AO15-AO$7</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS15" s="1"/>
+      <c r="AT15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU15" s="2">
+        <v>-2</v>
+      </c>
+      <c r="AW15" s="4">
+        <f>AU15-AU$7</f>
+        <v>4</v>
+      </c>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA15" s="2">
+        <v>-407</v>
+      </c>
+      <c r="BC15" s="4">
+        <f>BA15-BA$7</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
@@ -1263,8 +1482,10 @@
       <c r="AA16" s="1"/>
       <c r="AG16" s="1"/>
       <c r="AM16" s="1"/>
-    </row>
-    <row r="17" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS16" s="1"/>
+      <c r="AY16" s="1"/>
+    </row>
+    <row r="17" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>2</v>
@@ -1334,8 +1555,30 @@
         <f>AO17-AO$5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS17" s="1"/>
+      <c r="AT17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU17" s="2">
+        <v>1085</v>
+      </c>
+      <c r="AW17" s="4">
+        <f>AU17-AU$5</f>
+        <v>15</v>
+      </c>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA17" s="2">
+        <v>1420</v>
+      </c>
+      <c r="BC17" s="4">
+        <f>BA17-BA$5</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1446,8 +1689,40 @@
         <f>AO18-AO$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU18" s="2">
+        <v>75</v>
+      </c>
+      <c r="AV18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW18" s="4">
+        <f>AU18-AU$6</f>
+        <v>2</v>
+      </c>
+      <c r="AY18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA18" s="2">
+        <v>86</v>
+      </c>
+      <c r="BB18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC18" s="4">
+        <f>BA18-BA$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
         <v>4</v>
@@ -1517,11 +1792,35 @@
         <f>AO19-AO$7</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS19" s="1"/>
+      <c r="AT19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU19" s="2">
+        <v>-3</v>
+      </c>
+      <c r="AW19" s="4">
+        <f>AU19-AU$7</f>
+        <v>3</v>
+      </c>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA19" s="2">
+        <v>-425</v>
+      </c>
+      <c r="BC19" s="4">
+        <f>BA19-BA$7</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS20" s="1"/>
+      <c r="AY20" s="1"/>
+    </row>
+    <row r="21" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" t="s">
         <v>2</v>
@@ -1553,8 +1852,30 @@
         <f>AO21-AO$5</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS21" s="1"/>
+      <c r="AT21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU21" s="2">
+        <v>1074</v>
+      </c>
+      <c r="AW21" s="4">
+        <f>AU21-AU$5</f>
+        <v>4</v>
+      </c>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA21" s="2">
+        <v>1471</v>
+      </c>
+      <c r="BC21" s="4">
+        <f>BA21-BA$5</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1605,8 +1926,40 @@
         <f>AO22-AO$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AS22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU22" s="2">
+        <v>75</v>
+      </c>
+      <c r="AV22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW22" s="4">
+        <f>AU22-AU$6</f>
+        <v>2</v>
+      </c>
+      <c r="AY22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ22" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA22" s="2">
+        <v>86</v>
+      </c>
+      <c r="BB22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC22" s="4">
+        <f>BA22-BA$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:55" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -1637,8 +1990,28 @@
         <f>AO23-AO$7</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="3:43" x14ac:dyDescent="0.25">
+      <c r="AT23" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU23" s="2">
+        <v>7</v>
+      </c>
+      <c r="AW23" s="4">
+        <f>AU23-AU$7</f>
+        <v>13</v>
+      </c>
+      <c r="AZ23" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA23" s="2">
+        <v>-385</v>
+      </c>
+      <c r="BC23" s="4">
+        <f>BA23-BA$7</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="3:55" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
         <v>2</v>
       </c>
@@ -1660,7 +2033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:55" x14ac:dyDescent="0.25">
       <c r="AA26" s="1" t="s">
         <v>14</v>
       </c>
@@ -1695,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:55" x14ac:dyDescent="0.25">
       <c r="AB27" t="s">
         <v>4</v>
       </c>
@@ -1717,7 +2090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:55" x14ac:dyDescent="0.25">
       <c r="AN29" t="s">
         <v>2</v>
       </c>
@@ -1729,7 +2102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:55" x14ac:dyDescent="0.25">
       <c r="AM30" s="1" t="s">
         <v>21</v>
       </c>
@@ -1747,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:55" x14ac:dyDescent="0.25">
       <c r="AN31" t="s">
         <v>4</v>
       </c>
@@ -1844,7 +2217,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="AS3:AW3"/>
+    <mergeCell ref="AY3:BC3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="AA3:AE3"/>
     <mergeCell ref="AM3:AQ3"/>

</xml_diff>

<commit_message>
Tested moving platform and added test room to config
</commit_message>
<xml_diff>
--- a/Server_files/plugins/DunGen/Module_Coordinates.xlsx
+++ b/Server_files/plugins/DunGen/Module_Coordinates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="41">
   <si>
     <t>Raum mit Säulen</t>
   </si>
@@ -103,6 +103,45 @@
   </si>
   <si>
     <t>mazeCor2</t>
+  </si>
+  <si>
+    <t>movingPlatfTest</t>
+  </si>
+  <si>
+    <t>target1</t>
+  </si>
+  <si>
+    <t>target2</t>
+  </si>
+  <si>
+    <t>spawn1_1</t>
+  </si>
+  <si>
+    <t>spawn1_2</t>
+  </si>
+  <si>
+    <t>spawn2_2</t>
+  </si>
+  <si>
+    <t>spawn2_1</t>
+  </si>
+  <si>
+    <t>spawn3_1</t>
+  </si>
+  <si>
+    <t>spawn3_2</t>
+  </si>
+  <si>
+    <t>appear1</t>
+  </si>
+  <si>
+    <t>appear2</t>
+  </si>
+  <si>
+    <t>disap1</t>
+  </si>
+  <si>
+    <t>disap2</t>
   </si>
 </sst>
 </file>
@@ -494,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:BI40"/>
+  <dimension ref="C3:BO67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BG13" sqref="BG13"/>
+    <sheetView tabSelected="1" topLeftCell="BD37" workbookViewId="0">
+      <selection activeCell="BH52" sqref="BH52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +544,7 @@
     <col min="27" max="27" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -576,8 +615,15 @@
       <c r="BG3" s="5"/>
       <c r="BH3" s="5"/>
       <c r="BI3" s="5"/>
-    </row>
-    <row r="5" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL3" s="5"/>
+      <c r="BM3" s="5"/>
+      <c r="BN3" s="5"/>
+      <c r="BO3" s="5"/>
+    </row>
+    <row r="5" spans="3:67" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -636,8 +682,14 @@
       <c r="BG5" s="2">
         <v>957</v>
       </c>
-    </row>
-    <row r="6" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BL5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM5" s="2">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="6" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,8 +788,18 @@
         <v>63</v>
       </c>
       <c r="BH6" s="3"/>
-    </row>
-    <row r="7" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM6" s="2">
+        <v>64</v>
+      </c>
+      <c r="BN6" s="3"/>
+    </row>
+    <row r="7" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>4</v>
@@ -806,8 +868,15 @@
       <c r="BG7" s="2">
         <v>-246</v>
       </c>
-    </row>
-    <row r="8" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK7" s="1"/>
+      <c r="BL7" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM7" s="2">
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="8" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
@@ -818,8 +887,9 @@
       <c r="AS8" s="1"/>
       <c r="AY8" s="1"/>
       <c r="BE8" s="1"/>
-    </row>
-    <row r="9" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK8" s="1"/>
+    </row>
+    <row r="9" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>2</v>
@@ -928,8 +998,19 @@
         <f>BG9-BG$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK9" s="1"/>
+      <c r="BL9" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM9" s="2">
+        <v>1005</v>
+      </c>
+      <c r="BO9" s="4">
+        <f>BM9-BM$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1088,8 +1169,24 @@
         <f>BG10-BG$6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM10" s="2">
+        <v>67</v>
+      </c>
+      <c r="BN10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO10" s="4">
+        <f>BM10-BM$6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>4</v>
@@ -1198,8 +1295,19 @@
         <f>BG11-BG$7</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK11" s="1"/>
+      <c r="BL11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM11" s="2">
+        <v>-243</v>
+      </c>
+      <c r="BO11" s="4">
+        <f>BM11-BM$7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
@@ -1210,8 +1318,9 @@
       <c r="AS12" s="1"/>
       <c r="AY12" s="1"/>
       <c r="BE12" s="1"/>
-    </row>
-    <row r="13" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK12" s="1"/>
+    </row>
+    <row r="13" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>2</v>
@@ -1320,8 +1429,19 @@
         <f>BG13-BG$5</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK13" s="1"/>
+      <c r="BL13" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM13" s="2">
+        <v>1049</v>
+      </c>
+      <c r="BO13" s="4">
+        <f>BM13-BM$5</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1480,8 +1600,24 @@
         <f>BG14-BG$6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM14" s="2">
+        <v>67</v>
+      </c>
+      <c r="BN14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO14" s="4">
+        <f>BM14-BM$6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>4</v>
@@ -1590,8 +1726,19 @@
         <f>BG15-BG$7</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK15" s="1"/>
+      <c r="BL15" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM15" s="2">
+        <v>-243</v>
+      </c>
+      <c r="BO15" s="4">
+        <f>BM15-BM$7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
@@ -1602,8 +1749,9 @@
       <c r="AS16" s="1"/>
       <c r="AY16" s="1"/>
       <c r="BE16" s="1"/>
-    </row>
-    <row r="17" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK16" s="1"/>
+    </row>
+    <row r="17" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>2</v>
@@ -1704,8 +1852,19 @@
         <f>BG17-BG$5</f>
         <v>-957</v>
       </c>
-    </row>
-    <row r="18" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK17" s="1"/>
+      <c r="BL17" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM17" s="2">
+        <v>1045</v>
+      </c>
+      <c r="BO17" s="4">
+        <f>BM17-BM$5</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1862,8 +2021,24 @@
         <f>BG18-BG$6</f>
         <v>-63</v>
       </c>
-    </row>
-    <row r="19" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM18" s="2">
+        <v>66</v>
+      </c>
+      <c r="BN18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO18" s="4">
+        <f>BM18-BM$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
         <v>4</v>
@@ -1964,14 +2139,26 @@
         <f>BG19-BG$7</f>
         <v>246</v>
       </c>
-    </row>
-    <row r="20" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK19" s="1"/>
+      <c r="BL19" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM19" s="2">
+        <v>-242</v>
+      </c>
+      <c r="BO19" s="4">
+        <f>BM19-BM$7</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="AS20" s="1"/>
       <c r="AY20" s="1"/>
       <c r="BE20" s="1"/>
-    </row>
-    <row r="21" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK20" s="1"/>
+    </row>
+    <row r="21" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" t="s">
         <v>2</v>
@@ -2034,8 +2221,19 @@
         <f>BG21-BG$5</f>
         <v>-957</v>
       </c>
-    </row>
-    <row r="22" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK21" s="1"/>
+      <c r="BL21" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM21" s="2">
+        <v>1048</v>
+      </c>
+      <c r="BO21" s="4">
+        <f>BM21-BM$5</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="3:67" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
@@ -2132,8 +2330,24 @@
         <f>BG22-BG$6</f>
         <v>-63</v>
       </c>
-    </row>
-    <row r="23" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BL22" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM22" s="2">
+        <v>67</v>
+      </c>
+      <c r="BN22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO22" s="4">
+        <f>BM22-BM$6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:67" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -2192,8 +2406,18 @@
         <f>BG23-BG$7</f>
         <v>246</v>
       </c>
-    </row>
-    <row r="25" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BL23" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM23" s="2">
+        <v>-244</v>
+      </c>
+      <c r="BO23" s="4">
+        <f>BM23-BM$7</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="3:67" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
         <v>2</v>
       </c>
@@ -2224,8 +2448,18 @@
         <f>BG25-BG$5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BL25" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM25" s="2">
+        <v>1027</v>
+      </c>
+      <c r="BO25" s="4">
+        <f>BM25-BM$5</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="3:67" x14ac:dyDescent="0.25">
       <c r="AA26" s="1" t="s">
         <v>14</v>
       </c>
@@ -2275,8 +2509,24 @@
         <f>BG26-BG$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BL26" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM26" s="2">
+        <v>67</v>
+      </c>
+      <c r="BN26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO26" s="4">
+        <f>BM26-BM$6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:67" x14ac:dyDescent="0.25">
       <c r="AB27" t="s">
         <v>4</v>
       </c>
@@ -2307,8 +2557,18 @@
         <f>BG27-BG$7</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BL27" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM27" s="2">
+        <v>-240</v>
+      </c>
+      <c r="BO27" s="4">
+        <f>BM27-BM$7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="3:67" x14ac:dyDescent="0.25">
       <c r="AN29" t="s">
         <v>2</v>
       </c>
@@ -2329,8 +2589,18 @@
         <f>BG29-BG$5</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BL29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM29" s="2">
+        <v>1024</v>
+      </c>
+      <c r="BO29" s="4">
+        <f>BM29-BM$5</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="3:67" x14ac:dyDescent="0.25">
       <c r="AM30" s="1" t="s">
         <v>21</v>
       </c>
@@ -2363,8 +2633,24 @@
         <f>BG30-BG$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="3:61" x14ac:dyDescent="0.25">
+      <c r="BK30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BL30" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM30" s="2">
+        <v>67</v>
+      </c>
+      <c r="BN30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO30" s="4">
+        <f>BM30-BM$6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:67" x14ac:dyDescent="0.25">
       <c r="AN31" t="s">
         <v>4</v>
       </c>
@@ -2385,8 +2671,18 @@
         <f>BG31-BG$7</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="39:61" x14ac:dyDescent="0.25">
+      <c r="BL31" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM31" s="2">
+        <v>-238</v>
+      </c>
+      <c r="BO31" s="4">
+        <f>BM31-BM$7</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="39:67" x14ac:dyDescent="0.25">
       <c r="AN34" t="s">
         <v>2</v>
       </c>
@@ -2407,8 +2703,18 @@
         <f>BG34-BG$5</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="39:61" x14ac:dyDescent="0.25">
+      <c r="BL34" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM34" s="2">
+        <v>1032</v>
+      </c>
+      <c r="BO34" s="4">
+        <f>BM34-BM$5</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="39:67" x14ac:dyDescent="0.25">
       <c r="AM35" s="1" t="s">
         <v>22</v>
       </c>
@@ -2441,8 +2747,24 @@
         <f>BG35-BG$6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="39:61" x14ac:dyDescent="0.25">
+      <c r="BK35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BL35" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM35" s="2">
+        <v>66</v>
+      </c>
+      <c r="BN35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO35" s="4">
+        <f>BM35-BM$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="39:67" x14ac:dyDescent="0.25">
       <c r="AN36" t="s">
         <v>4</v>
       </c>
@@ -2463,8 +2785,18 @@
         <f>BG36-BG$7</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="39:61" x14ac:dyDescent="0.25">
+      <c r="BL36" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM36" s="2">
+        <v>-245</v>
+      </c>
+      <c r="BO36" s="4">
+        <f>BM36-BM$7</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="39:67" x14ac:dyDescent="0.25">
       <c r="AN38" t="s">
         <v>2</v>
       </c>
@@ -2485,8 +2817,18 @@
         <f>BG38-BG$5</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="39:61" x14ac:dyDescent="0.25">
+      <c r="BL38" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM38" s="2">
+        <v>1033</v>
+      </c>
+      <c r="BO38" s="4">
+        <f>BM38-BM$5</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="39:67" x14ac:dyDescent="0.25">
       <c r="AM39" s="1" t="s">
         <v>23</v>
       </c>
@@ -2519,8 +2861,24 @@
         <f>BG39-BG$6</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="39:61" x14ac:dyDescent="0.25">
+      <c r="BK39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BL39" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM39" s="2">
+        <v>66</v>
+      </c>
+      <c r="BN39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO39" s="4">
+        <f>BM39-BM$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="39:67" x14ac:dyDescent="0.25">
       <c r="AN40" t="s">
         <v>4</v>
       </c>
@@ -2541,9 +2899,272 @@
         <f>BG40-BG$7</f>
         <v>14</v>
       </c>
+      <c r="BL40" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM40" s="2">
+        <v>-249</v>
+      </c>
+      <c r="BO40" s="4">
+        <f>BM40-BM$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BL43" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM43" s="2">
+        <v>1040</v>
+      </c>
+      <c r="BO43" s="4">
+        <f>BM43-BM$5</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BK44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BL44" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM44" s="2">
+        <v>68</v>
+      </c>
+      <c r="BN44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO44" s="4">
+        <f>BM44-BM$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BL45" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM45" s="2">
+        <v>-240</v>
+      </c>
+      <c r="BO45" s="4">
+        <f>BM45-BM$7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BL47" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM47" s="2">
+        <v>1041</v>
+      </c>
+      <c r="BO47" s="4">
+        <f>BM47-BM$5</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BK48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BL48" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM48" s="2">
+        <v>68</v>
+      </c>
+      <c r="BN48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO48" s="4">
+        <f>BM48-BM$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL49" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM49" s="2">
+        <v>-238</v>
+      </c>
+      <c r="BO49" s="4">
+        <f>BM49-BM$7</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL52" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM52" s="2">
+        <v>1015</v>
+      </c>
+      <c r="BO52" s="4">
+        <f>BM52-BM$5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BK53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BL53" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM53" s="2">
+        <v>66</v>
+      </c>
+      <c r="BN53" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO53" s="4">
+        <f>BM53-BM$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL54" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM54" s="2">
+        <v>-244</v>
+      </c>
+      <c r="BO54" s="4">
+        <f>BM54-BM$7</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL56" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM56" s="2">
+        <v>1015</v>
+      </c>
+      <c r="BO56" s="4">
+        <f>BM56-BM$5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BK57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL57" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM57" s="2">
+        <v>66</v>
+      </c>
+      <c r="BN57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO57" s="4">
+        <f>BM57-BM$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL58" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM58" s="2">
+        <v>-241</v>
+      </c>
+      <c r="BO58" s="4">
+        <f>BM58-BM$7</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL61" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM61" s="2">
+        <v>1009</v>
+      </c>
+      <c r="BO61" s="4">
+        <f>BM61-BM$5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BK62" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BL62" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM62" s="2">
+        <v>66</v>
+      </c>
+      <c r="BN62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO62" s="4">
+        <f>BM62-BM$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL63" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM63" s="2">
+        <v>-244</v>
+      </c>
+      <c r="BO63" s="4">
+        <f>BM63-BM$7</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL65" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM65" s="2">
+        <v>1009</v>
+      </c>
+      <c r="BO65" s="4">
+        <f>BM65-BM$5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BK66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BL66" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM66" s="2">
+        <v>66</v>
+      </c>
+      <c r="BN66" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO66" s="4">
+        <f>BM66-BM$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="63:67" x14ac:dyDescent="0.25">
+      <c r="BL67" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM67" s="2">
+        <v>-241</v>
+      </c>
+      <c r="BO67" s="4">
+        <f>BM67-BM$7</f>
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="BK3:BO3"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="AS3:AW3"/>
     <mergeCell ref="AY3:BC3"/>

</xml_diff>

<commit_message>
Initial implementation, test and debug! Also add hole mode.
</commit_message>
<xml_diff>
--- a/Server_files/plugins/DunGen/Module_Coordinates.xlsx
+++ b/Server_files/plugins/DunGen/Module_Coordinates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="45">
   <si>
     <t>Raum mit Säulen</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>disap2</t>
+  </si>
+  <si>
+    <t>adaptiveMazeTest</t>
+  </si>
+  <si>
+    <t>maze cell size width</t>
+  </si>
+  <si>
+    <t>maze cell size height</t>
+  </si>
+  <si>
+    <t>entryCell (width)</t>
   </si>
 </sst>
 </file>
@@ -533,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:BO67"/>
+  <dimension ref="C3:BU67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD37" workbookViewId="0">
-      <selection activeCell="BH52" sqref="BH52"/>
+    <sheetView tabSelected="1" topLeftCell="BH22" workbookViewId="0">
+      <selection activeCell="BT45" sqref="BT45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +556,7 @@
     <col min="27" max="27" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:67" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -622,8 +634,15 @@
       <c r="BM3" s="5"/>
       <c r="BN3" s="5"/>
       <c r="BO3" s="5"/>
-    </row>
-    <row r="5" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="BR3" s="5"/>
+      <c r="BS3" s="5"/>
+      <c r="BT3" s="5"/>
+      <c r="BU3" s="5"/>
+    </row>
+    <row r="5" spans="3:73" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -688,8 +707,14 @@
       <c r="BM5" s="2">
         <v>1005</v>
       </c>
-    </row>
-    <row r="6" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BR5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS5" s="2">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="6" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -798,8 +823,18 @@
         <v>64</v>
       </c>
       <c r="BN6" s="3"/>
-    </row>
-    <row r="7" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS6" s="2">
+        <v>97</v>
+      </c>
+      <c r="BT6" s="3"/>
+    </row>
+    <row r="7" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>4</v>
@@ -875,8 +910,15 @@
       <c r="BM7" s="2">
         <v>-250</v>
       </c>
-    </row>
-    <row r="8" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ7" s="1"/>
+      <c r="BR7" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS7" s="2">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="8" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
@@ -888,8 +930,9 @@
       <c r="AY8" s="1"/>
       <c r="BE8" s="1"/>
       <c r="BK8" s="1"/>
-    </row>
-    <row r="9" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ8" s="1"/>
+    </row>
+    <row r="9" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>2</v>
@@ -1009,8 +1052,19 @@
         <f>BM9-BM$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ9" s="1"/>
+      <c r="BR9" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS9" s="2">
+        <v>959</v>
+      </c>
+      <c r="BU9" s="4">
+        <f>BS9-BS$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1185,8 +1239,24 @@
         <f>BM10-BM$6</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS10" s="2">
+        <v>98</v>
+      </c>
+      <c r="BT10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU10" s="4">
+        <f>BS10-BS$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>4</v>
@@ -1306,8 +1376,19 @@
         <f>BM11-BM$7</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ11" s="1"/>
+      <c r="BR11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS11" s="2">
+        <v>-130</v>
+      </c>
+      <c r="BU11" s="4">
+        <f>BS11-BS$7</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
@@ -1319,8 +1400,9 @@
       <c r="AY12" s="1"/>
       <c r="BE12" s="1"/>
       <c r="BK12" s="1"/>
-    </row>
-    <row r="13" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ12" s="1"/>
+    </row>
+    <row r="13" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>2</v>
@@ -1440,8 +1522,19 @@
         <f>BM13-BM$5</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ13" s="1"/>
+      <c r="BR13" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS13" s="2">
+        <v>1002</v>
+      </c>
+      <c r="BU13" s="4">
+        <f>BS13-BS$5</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1616,8 +1709,24 @@
         <f>BM14-BM$6</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS14" s="2">
+        <v>98</v>
+      </c>
+      <c r="BT14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU14" s="4">
+        <f>BS14-BS$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>4</v>
@@ -1737,8 +1846,19 @@
         <f>BM15-BM$7</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ15" s="1"/>
+      <c r="BR15" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS15" s="2">
+        <v>-130</v>
+      </c>
+      <c r="BU15" s="4">
+        <f>BS15-BS$7</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
@@ -1750,8 +1870,9 @@
       <c r="AY16" s="1"/>
       <c r="BE16" s="1"/>
       <c r="BK16" s="1"/>
-    </row>
-    <row r="17" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ16" s="1"/>
+    </row>
+    <row r="17" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>2</v>
@@ -1863,8 +1984,17 @@
         <f>BM17-BM$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ17" s="1"/>
+      <c r="BR17" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS17" s="2"/>
+      <c r="BU17" s="4">
+        <f>BS17-BS$5</f>
+        <v>-959</v>
+      </c>
+    </row>
+    <row r="18" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2037,8 +2167,22 @@
         <f>BM18-BM$6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR18" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS18" s="2"/>
+      <c r="BT18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU18" s="4">
+        <f>BS18-BS$6</f>
+        <v>-97</v>
+      </c>
+    </row>
+    <row r="19" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
         <v>4</v>
@@ -2150,15 +2294,25 @@
         <f>BM19-BM$7</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ19" s="1"/>
+      <c r="BR19" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS19" s="2"/>
+      <c r="BU19" s="4">
+        <f>BS19-BS$7</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="AS20" s="1"/>
       <c r="AY20" s="1"/>
       <c r="BE20" s="1"/>
       <c r="BK20" s="1"/>
-    </row>
-    <row r="21" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ20" s="1"/>
+    </row>
+    <row r="21" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" t="s">
         <v>2</v>
@@ -2232,8 +2386,17 @@
         <f>BM21-BM$5</f>
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ21" s="1"/>
+      <c r="BR21" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS21" s="2"/>
+      <c r="BU21" s="4">
+        <f>BS21-BS$5</f>
+        <v>-959</v>
+      </c>
+    </row>
+    <row r="22" spans="3:73" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
@@ -2346,8 +2509,22 @@
         <f>BM22-BM$6</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR22" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS22" s="2"/>
+      <c r="BT22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU22" s="4">
+        <f>BS22-BS$6</f>
+        <v>-97</v>
+      </c>
+    </row>
+    <row r="23" spans="3:73" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -2416,8 +2593,16 @@
         <f>BM23-BM$7</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BR23" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS23" s="2"/>
+      <c r="BU23" s="4">
+        <f>BS23-BS$7</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="3:73" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
         <v>2</v>
       </c>
@@ -2458,8 +2643,18 @@
         <f>BM25-BM$5</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BR25" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS25" s="2">
+        <v>960</v>
+      </c>
+      <c r="BU25" s="4">
+        <f>BS25-BS$5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:73" x14ac:dyDescent="0.25">
       <c r="AA26" s="1" t="s">
         <v>14</v>
       </c>
@@ -2525,8 +2720,24 @@
         <f>BM26-BM$6</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BR26" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS26" s="2">
+        <v>98</v>
+      </c>
+      <c r="BT26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU26" s="4">
+        <f>BS26-BS$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:73" x14ac:dyDescent="0.25">
       <c r="AB27" t="s">
         <v>4</v>
       </c>
@@ -2567,8 +2778,18 @@
         <f>BM27-BM$7</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BR27" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS27" s="2">
+        <v>-146</v>
+      </c>
+      <c r="BU27" s="4">
+        <f>BS27-BS$7</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="3:73" x14ac:dyDescent="0.25">
       <c r="AN29" t="s">
         <v>2</v>
       </c>
@@ -2599,8 +2820,18 @@
         <f>BM29-BM$5</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BR29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS29" s="2">
+        <v>997</v>
+      </c>
+      <c r="BU29" s="4">
+        <f>BS29-BS$5</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="3:73" x14ac:dyDescent="0.25">
       <c r="AM30" s="1" t="s">
         <v>21</v>
       </c>
@@ -2649,8 +2880,24 @@
         <f>BM30-BM$6</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="3:67" x14ac:dyDescent="0.25">
+      <c r="BQ30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BR30" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS30" s="2">
+        <v>98</v>
+      </c>
+      <c r="BT30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU30" s="4">
+        <f>BS30-BS$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:73" x14ac:dyDescent="0.25">
       <c r="AN31" t="s">
         <v>4</v>
       </c>
@@ -2681,8 +2928,18 @@
         <f>BM31-BM$7</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BR31" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS31" s="2">
+        <v>-113</v>
+      </c>
+      <c r="BU31" s="4">
+        <f>BS31-BS$7</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="39:73" x14ac:dyDescent="0.25">
       <c r="AN34" t="s">
         <v>2</v>
       </c>
@@ -2713,8 +2970,18 @@
         <f>BM34-BM$5</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BR34" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS34" s="2">
+        <v>1001</v>
+      </c>
+      <c r="BU34" s="4">
+        <f>BS34-BS$5</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="39:73" x14ac:dyDescent="0.25">
       <c r="AM35" s="1" t="s">
         <v>22</v>
       </c>
@@ -2763,8 +3030,24 @@
         <f>BM35-BM$6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BQ35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BR35" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS35" s="2">
+        <v>98</v>
+      </c>
+      <c r="BT35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU35" s="4">
+        <f>BS35-BS$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="39:73" x14ac:dyDescent="0.25">
       <c r="AN36" t="s">
         <v>4</v>
       </c>
@@ -2795,8 +3078,18 @@
         <f>BM36-BM$7</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BR36" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS36" s="2">
+        <v>-132</v>
+      </c>
+      <c r="BU36" s="4">
+        <f>BS36-BS$7</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="39:73" x14ac:dyDescent="0.25">
       <c r="AN38" t="s">
         <v>2</v>
       </c>
@@ -2827,8 +3120,18 @@
         <f>BM38-BM$5</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BR38" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS38" s="2">
+        <v>999</v>
+      </c>
+      <c r="BU38" s="4">
+        <f>BS38-BS$5</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="39:73" x14ac:dyDescent="0.25">
       <c r="AM39" s="1" t="s">
         <v>23</v>
       </c>
@@ -2877,8 +3180,24 @@
         <f>BM39-BM$6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BQ39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR39" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS39" s="2">
+        <v>99</v>
+      </c>
+      <c r="BT39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU39" s="4">
+        <f>BS39-BS$6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="39:73" x14ac:dyDescent="0.25">
       <c r="AN40" t="s">
         <v>4</v>
       </c>
@@ -2909,8 +3228,26 @@
         <f>BM40-BM$7</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BR40" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS40" s="2">
+        <v>-127</v>
+      </c>
+      <c r="BU40" s="4">
+        <f>BS40-BS$7</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BQ42" t="s">
+        <v>42</v>
+      </c>
+      <c r="BT42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="39:73" x14ac:dyDescent="0.25">
       <c r="BL43" t="s">
         <v>2</v>
       </c>
@@ -2922,7 +3259,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="39:67" x14ac:dyDescent="0.25">
+    <row r="44" spans="39:73" x14ac:dyDescent="0.25">
       <c r="BK44" s="1" t="s">
         <v>35</v>
       </c>
@@ -2939,8 +3276,14 @@
         <f>BM44-BM$6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="39:67" x14ac:dyDescent="0.25">
+      <c r="BQ44" t="s">
+        <v>43</v>
+      </c>
+      <c r="BT44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="39:73" x14ac:dyDescent="0.25">
       <c r="BL45" t="s">
         <v>4</v>
       </c>
@@ -2952,7 +3295,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="39:67" x14ac:dyDescent="0.25">
+    <row r="46" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BQ46" t="s">
+        <v>44</v>
+      </c>
+      <c r="BT46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="39:73" x14ac:dyDescent="0.25">
       <c r="BL47" t="s">
         <v>2</v>
       </c>
@@ -2964,7 +3315,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="39:67" x14ac:dyDescent="0.25">
+    <row r="48" spans="39:73" x14ac:dyDescent="0.25">
       <c r="BK48" s="1" t="s">
         <v>36</v>
       </c>
@@ -3163,7 +3514,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="BQ3:BU3"/>
     <mergeCell ref="BK3:BO3"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="AS3:AW3"/>

</xml_diff>

<commit_message>
Tested, ready to merge :)
</commit_message>
<xml_diff>
--- a/Server_files/plugins/DunGen/Module_Coordinates.xlsx
+++ b/Server_files/plugins/DunGen/Module_Coordinates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="45">
   <si>
     <t>Raum mit Säulen</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:BU67"/>
+  <dimension ref="C3:CA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH22" workbookViewId="0">
-      <selection activeCell="BT45" sqref="BT45"/>
+    <sheetView tabSelected="1" topLeftCell="BG4" workbookViewId="0">
+      <selection activeCell="CC15" sqref="CC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +556,7 @@
     <col min="27" max="27" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:73" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -641,8 +641,15 @@
       <c r="BS3" s="5"/>
       <c r="BT3" s="5"/>
       <c r="BU3" s="5"/>
-    </row>
-    <row r="5" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="BX3" s="5"/>
+      <c r="BY3" s="5"/>
+      <c r="BZ3" s="5"/>
+      <c r="CA3" s="5"/>
+    </row>
+    <row r="5" spans="3:79" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -713,8 +720,14 @@
       <c r="BS5" s="2">
         <v>959</v>
       </c>
-    </row>
-    <row r="6" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BX5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY5" s="2">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="6" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -833,8 +846,18 @@
         <v>97</v>
       </c>
       <c r="BT6" s="3"/>
-    </row>
-    <row r="7" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY6" s="2">
+        <v>76</v>
+      </c>
+      <c r="BZ6" s="3"/>
+    </row>
+    <row r="7" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>4</v>
@@ -917,8 +940,15 @@
       <c r="BS7" s="2">
         <v>-150</v>
       </c>
-    </row>
-    <row r="8" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW7" s="1"/>
+      <c r="BX7" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY7" s="2">
+        <v>-303</v>
+      </c>
+    </row>
+    <row r="8" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="I8" s="1"/>
       <c r="O8" s="1"/>
@@ -931,8 +961,9 @@
       <c r="BE8" s="1"/>
       <c r="BK8" s="1"/>
       <c r="BQ8" s="1"/>
-    </row>
-    <row r="9" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW8" s="1"/>
+    </row>
+    <row r="9" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>2</v>
@@ -1063,8 +1094,19 @@
         <f>BS9-BS$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW9" s="1"/>
+      <c r="BX9" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY9" s="2">
+        <v>952</v>
+      </c>
+      <c r="CA9" s="4">
+        <f>BY9-BY$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1255,8 +1297,24 @@
         <f>BS10-BS$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BX10" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY10" s="2">
+        <v>84</v>
+      </c>
+      <c r="BZ10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA10" s="4">
+        <f>BY10-BY$6</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>4</v>
@@ -1387,8 +1445,19 @@
         <f>BS11-BS$7</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW11" s="1"/>
+      <c r="BX11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY11" s="2">
+        <v>-292</v>
+      </c>
+      <c r="CA11" s="4">
+        <f>BY11-BY$7</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="I12" s="1"/>
       <c r="O12" s="1"/>
@@ -1401,8 +1470,9 @@
       <c r="BE12" s="1"/>
       <c r="BK12" s="1"/>
       <c r="BQ12" s="1"/>
-    </row>
-    <row r="13" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW12" s="1"/>
+    </row>
+    <row r="13" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>2</v>
@@ -1533,8 +1603,19 @@
         <f>BS13-BS$5</f>
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW13" s="1"/>
+      <c r="BX13" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY13" s="2">
+        <v>963</v>
+      </c>
+      <c r="CA13" s="4">
+        <f>BY13-BY$5</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1725,8 +1806,24 @@
         <f>BS14-BS$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BX14" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY14" s="2">
+        <v>79</v>
+      </c>
+      <c r="BZ14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA14" s="4">
+        <f>BY14-BY$6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>4</v>
@@ -1857,8 +1954,19 @@
         <f>BS15-BS$7</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW15" s="1"/>
+      <c r="BX15" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY15" s="2">
+        <v>-303</v>
+      </c>
+      <c r="CA15" s="4">
+        <f>BY15-BY$7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="I16" s="1"/>
       <c r="O16" s="1"/>
@@ -1871,8 +1979,9 @@
       <c r="BE16" s="1"/>
       <c r="BK16" s="1"/>
       <c r="BQ16" s="1"/>
-    </row>
-    <row r="17" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW16" s="1"/>
+    </row>
+    <row r="17" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" t="s">
         <v>2</v>
@@ -1993,8 +2102,11 @@
         <f>BS17-BS$5</f>
         <v>-959</v>
       </c>
-    </row>
-    <row r="18" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW17" s="1"/>
+      <c r="BY17" s="2"/>
+      <c r="CA17" s="4"/>
+    </row>
+    <row r="18" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2181,8 +2293,12 @@
         <f>BS18-BS$6</f>
         <v>-97</v>
       </c>
-    </row>
-    <row r="19" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW18" s="1"/>
+      <c r="BY18" s="2"/>
+      <c r="BZ18" s="3"/>
+      <c r="CA18" s="4"/>
+    </row>
+    <row r="19" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" t="s">
         <v>4</v>
@@ -2303,16 +2419,20 @@
         <f>BS19-BS$7</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="20" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW19" s="1"/>
+      <c r="BY19" s="2"/>
+      <c r="CA19" s="4"/>
+    </row>
+    <row r="20" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="AS20" s="1"/>
       <c r="AY20" s="1"/>
       <c r="BE20" s="1"/>
       <c r="BK20" s="1"/>
       <c r="BQ20" s="1"/>
-    </row>
-    <row r="21" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW20" s="1"/>
+    </row>
+    <row r="21" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" t="s">
         <v>2</v>
@@ -2395,8 +2515,11 @@
         <f>BS21-BS$5</f>
         <v>-959</v>
       </c>
-    </row>
-    <row r="22" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW21" s="1"/>
+      <c r="BY21" s="2"/>
+      <c r="CA21" s="4"/>
+    </row>
+    <row r="22" spans="3:79" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
@@ -2523,8 +2646,12 @@
         <f>BS22-BS$6</f>
         <v>-97</v>
       </c>
-    </row>
-    <row r="23" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW22" s="1"/>
+      <c r="BY22" s="2"/>
+      <c r="BZ22" s="3"/>
+      <c r="CA22" s="4"/>
+    </row>
+    <row r="23" spans="3:79" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>4</v>
       </c>
@@ -2601,8 +2728,10 @@
         <f>BS23-BS$7</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BY23" s="2"/>
+      <c r="CA23" s="4"/>
+    </row>
+    <row r="25" spans="3:79" x14ac:dyDescent="0.25">
       <c r="AB25" t="s">
         <v>2</v>
       </c>
@@ -2653,8 +2782,18 @@
         <f>BS25-BS$5</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BX25" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY25" s="2">
+        <v>954</v>
+      </c>
+      <c r="CA25" s="4">
+        <f>BY25-BY$5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:79" x14ac:dyDescent="0.25">
       <c r="AA26" s="1" t="s">
         <v>14</v>
       </c>
@@ -2736,8 +2875,24 @@
         <f>BS26-BS$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BX26" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY26" s="2">
+        <v>83</v>
+      </c>
+      <c r="BZ26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA26" s="4">
+        <f>BY26-BY$6</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:79" x14ac:dyDescent="0.25">
       <c r="AB27" t="s">
         <v>4</v>
       </c>
@@ -2788,8 +2943,18 @@
         <f>BS27-BS$7</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BX27" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY27" s="2">
+        <v>-301</v>
+      </c>
+      <c r="CA27" s="4">
+        <f>BY27-BY$7</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:79" x14ac:dyDescent="0.25">
       <c r="AN29" t="s">
         <v>2</v>
       </c>
@@ -2830,8 +2995,18 @@
         <f>BS29-BS$5</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BX29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY29" s="2">
+        <v>973</v>
+      </c>
+      <c r="CA29" s="4">
+        <f>BY29-BY$5</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="3:79" x14ac:dyDescent="0.25">
       <c r="AM30" s="1" t="s">
         <v>21</v>
       </c>
@@ -2896,8 +3071,24 @@
         <f>BS30-BS$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="3:73" x14ac:dyDescent="0.25">
+      <c r="BW30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BX30" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY30" s="2">
+        <v>83</v>
+      </c>
+      <c r="BZ30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA30" s="4">
+        <f>BY30-BY$6</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="3:79" x14ac:dyDescent="0.25">
       <c r="AN31" t="s">
         <v>4</v>
       </c>
@@ -2938,8 +3129,18 @@
         <f>BS31-BS$7</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BX31" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY31" s="2">
+        <v>-282</v>
+      </c>
+      <c r="CA31" s="4">
+        <f>BY31-BY$7</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="39:79" x14ac:dyDescent="0.25">
       <c r="AN34" t="s">
         <v>2</v>
       </c>
@@ -2980,8 +3181,18 @@
         <f>BS34-BS$5</f>
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BX34" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY34" s="2">
+        <v>954</v>
+      </c>
+      <c r="CA34" s="4">
+        <f>BY34-BY$5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="39:79" x14ac:dyDescent="0.25">
       <c r="AM35" s="1" t="s">
         <v>22</v>
       </c>
@@ -3046,8 +3257,24 @@
         <f>BS35-BS$6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BW35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BX35" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY35" s="2">
+        <v>79</v>
+      </c>
+      <c r="BZ35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA35" s="4">
+        <f>BY35-BY$6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="39:79" x14ac:dyDescent="0.25">
       <c r="AN36" t="s">
         <v>4</v>
       </c>
@@ -3088,8 +3315,18 @@
         <f>BS36-BS$7</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BX36" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY36" s="2">
+        <v>-301</v>
+      </c>
+      <c r="CA36" s="4">
+        <f>BY36-BY$7</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="39:79" x14ac:dyDescent="0.25">
       <c r="AN38" t="s">
         <v>2</v>
       </c>
@@ -3130,8 +3367,18 @@
         <f>BS38-BS$5</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BX38" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY38" s="2">
+        <v>973</v>
+      </c>
+      <c r="CA38" s="4">
+        <f>BY38-BY$5</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="39:79" x14ac:dyDescent="0.25">
       <c r="AM39" s="1" t="s">
         <v>23</v>
       </c>
@@ -3196,8 +3443,24 @@
         <f>BS39-BS$6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BW39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BX39" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY39" s="2">
+        <v>80</v>
+      </c>
+      <c r="BZ39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="CA39" s="4">
+        <f>BY39-BY$6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="39:79" x14ac:dyDescent="0.25">
       <c r="AN40" t="s">
         <v>4</v>
       </c>
@@ -3238,8 +3501,18 @@
         <f>BS40-BS$7</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="39:73" x14ac:dyDescent="0.25">
+      <c r="BX40" t="s">
+        <v>4</v>
+      </c>
+      <c r="BY40" s="2">
+        <v>-282</v>
+      </c>
+      <c r="CA40" s="4">
+        <f>BY40-BY$7</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="39:79" x14ac:dyDescent="0.25">
       <c r="BQ42" t="s">
         <v>42</v>
       </c>
@@ -3247,7 +3520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="39:73" x14ac:dyDescent="0.25">
+    <row r="43" spans="39:79" x14ac:dyDescent="0.25">
       <c r="BL43" t="s">
         <v>2</v>
       </c>
@@ -3259,7 +3532,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="39:73" x14ac:dyDescent="0.25">
+    <row r="44" spans="39:79" x14ac:dyDescent="0.25">
       <c r="BK44" s="1" t="s">
         <v>35</v>
       </c>
@@ -3283,7 +3556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="39:73" x14ac:dyDescent="0.25">
+    <row r="45" spans="39:79" x14ac:dyDescent="0.25">
       <c r="BL45" t="s">
         <v>4</v>
       </c>
@@ -3295,7 +3568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="39:73" x14ac:dyDescent="0.25">
+    <row r="46" spans="39:79" x14ac:dyDescent="0.25">
       <c r="BQ46" t="s">
         <v>44</v>
       </c>
@@ -3303,7 +3576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="39:73" x14ac:dyDescent="0.25">
+    <row r="47" spans="39:79" x14ac:dyDescent="0.25">
       <c r="BL47" t="s">
         <v>2</v>
       </c>
@@ -3315,7 +3588,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="39:73" x14ac:dyDescent="0.25">
+    <row r="48" spans="39:79" x14ac:dyDescent="0.25">
       <c r="BK48" s="1" t="s">
         <v>36</v>
       </c>
@@ -3514,12 +3787,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="BQ3:BU3"/>
-    <mergeCell ref="BK3:BO3"/>
-    <mergeCell ref="BE3:BI3"/>
-    <mergeCell ref="AS3:AW3"/>
-    <mergeCell ref="AY3:BC3"/>
+  <mergeCells count="13">
+    <mergeCell ref="BW3:CA3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="AA3:AE3"/>
     <mergeCell ref="AM3:AQ3"/>
@@ -3527,6 +3796,11 @@
     <mergeCell ref="U3:Y3"/>
     <mergeCell ref="O3:S3"/>
     <mergeCell ref="I3:M3"/>
+    <mergeCell ref="BQ3:BU3"/>
+    <mergeCell ref="BK3:BO3"/>
+    <mergeCell ref="BE3:BI3"/>
+    <mergeCell ref="AS3:AW3"/>
+    <mergeCell ref="AY3:BC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>